<commit_message>
better dtg when manually diverting off route
</commit_message>
<xml_diff>
--- a/scenario/LVNL/Maps/T-bar/Waypoints.xlsx
+++ b/scenario/LVNL/Maps/T-bar/Waypoints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LVNL_ILAB3\PycharmProjects\bluesky\scenario\T-bar\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\bluesky_ilabs\scenario\LVNL\Maps\T-bar\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E18A3990-9489-4BCB-AF06-E95FB218DC54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F6C4C1E-05AE-4C1E-9FBF-FD50F9994DFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4840" yWindow="630" windowWidth="19200" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="70">
   <si>
     <t>Name</t>
   </si>
@@ -229,6 +229,12 @@
   </si>
   <si>
     <t>N 52:29:26.20E 05:23:47.62</t>
+  </si>
+  <si>
+    <t>NAAAR</t>
+  </si>
+  <si>
+    <t>N 52:00:00.00E 03:00:00.00</t>
   </si>
 </sst>
 </file>
@@ -268,7 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -546,19 +552,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -566,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -574,7 +580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -582,7 +588,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -590,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -598,7 +604,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -606,7 +612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>25</v>
       </c>
@@ -614,7 +620,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -622,7 +628,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>27</v>
       </c>
@@ -630,7 +636,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>28</v>
       </c>
@@ -638,7 +644,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>29</v>
       </c>
@@ -646,7 +652,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>30</v>
       </c>
@@ -654,7 +660,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>31</v>
       </c>
@@ -662,7 +668,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>32</v>
       </c>
@@ -670,7 +676,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>33</v>
       </c>
@@ -678,7 +684,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -686,7 +692,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -694,7 +700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -702,7 +708,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -710,7 +716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -718,7 +724,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -726,7 +732,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -734,7 +740,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>32</v>
       </c>
@@ -742,7 +748,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>41</v>
       </c>
@@ -750,7 +756,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>42</v>
       </c>
@@ -758,7 +764,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>43</v>
       </c>
@@ -766,7 +772,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -774,7 +780,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>44</v>
       </c>
@@ -782,7 +788,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -790,7 +796,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -798,7 +804,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>45</v>
       </c>
@@ -806,7 +812,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>33</v>
       </c>
@@ -814,7 +820,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -822,7 +828,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>35</v>
       </c>
@@ -830,7 +836,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>28</v>
       </c>
@@ -838,7 +844,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -846,7 +852,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>30</v>
       </c>
@@ -854,7 +860,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -862,7 +868,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>20</v>
       </c>
@@ -870,7 +876,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>21</v>
       </c>
@@ -878,7 +884,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -886,7 +892,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>35</v>
       </c>
@@ -894,7 +900,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>56</v>
       </c>
@@ -902,7 +908,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>57</v>
       </c>
@@ -910,7 +916,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>58</v>
       </c>
@@ -918,7 +924,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>36</v>
       </c>
@@ -926,7 +932,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>30</v>
       </c>
@@ -934,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>59</v>
       </c>
@@ -942,7 +948,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>33</v>
       </c>
@@ -950,7 +956,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>60</v>
       </c>
@@ -958,7 +964,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>37</v>
       </c>
@@ -966,7 +972,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>32</v>
       </c>
@@ -974,7 +980,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>34</v>
       </c>
@@ -982,7 +988,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>23</v>
       </c>
@@ -990,7 +996,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>28</v>
       </c>
@@ -998,12 +1004,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>27</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>68</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>